<commit_message>
Update rent sensitivity analysis parameters and adjust rent levels range
</commit_message>
<xml_diff>
--- a/rent_sensitivity_barking_riverside.xlsx
+++ b/rent_sensitivity_barking_riverside.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,19 +478,19 @@
         <v>300</v>
       </c>
       <c r="C2" t="n">
-        <v>1290</v>
+        <v>1318</v>
       </c>
       <c r="D2" t="n">
-        <v>516</v>
+        <v>527.2</v>
       </c>
       <c r="E2" t="n">
-        <v>103.2</v>
+        <v>105.44</v>
       </c>
       <c r="F2" t="n">
-        <v>353.2</v>
+        <v>366.64</v>
       </c>
       <c r="G2" t="n">
-        <v>-813.2</v>
+        <v>-798.64</v>
       </c>
     </row>
     <row r="3">
@@ -501,19 +501,19 @@
         <v>307.5</v>
       </c>
       <c r="C3" t="n">
-        <v>1332.5</v>
+        <v>1360.5</v>
       </c>
       <c r="D3" t="n">
-        <v>533</v>
+        <v>544.2</v>
       </c>
       <c r="E3" t="n">
-        <v>106.6</v>
+        <v>108.84</v>
       </c>
       <c r="F3" t="n">
-        <v>373.6</v>
+        <v>387.04</v>
       </c>
       <c r="G3" t="n">
-        <v>-791.1</v>
+        <v>-776.54</v>
       </c>
     </row>
     <row r="4">
@@ -524,19 +524,19 @@
         <v>315</v>
       </c>
       <c r="C4" t="n">
-        <v>1375</v>
+        <v>1403</v>
       </c>
       <c r="D4" t="n">
-        <v>550</v>
+        <v>561.2</v>
       </c>
       <c r="E4" t="n">
-        <v>110</v>
+        <v>112.24</v>
       </c>
       <c r="F4" t="n">
-        <v>394</v>
+        <v>407.44</v>
       </c>
       <c r="G4" t="n">
-        <v>-769</v>
+        <v>-754.4400000000001</v>
       </c>
     </row>
     <row r="5">
@@ -547,19 +547,19 @@
         <v>322.5</v>
       </c>
       <c r="C5" t="n">
-        <v>1417.5</v>
+        <v>1445.5</v>
       </c>
       <c r="D5" t="n">
-        <v>567</v>
+        <v>578.2</v>
       </c>
       <c r="E5" t="n">
-        <v>113.4</v>
+        <v>115.64</v>
       </c>
       <c r="F5" t="n">
-        <v>414.4</v>
+        <v>427.84</v>
       </c>
       <c r="G5" t="n">
-        <v>-746.9</v>
+        <v>-732.34</v>
       </c>
     </row>
     <row r="6">
@@ -570,19 +570,19 @@
         <v>330</v>
       </c>
       <c r="C6" t="n">
-        <v>1460</v>
+        <v>1488</v>
       </c>
       <c r="D6" t="n">
-        <v>584</v>
+        <v>595.2</v>
       </c>
       <c r="E6" t="n">
-        <v>116.8</v>
+        <v>119.04</v>
       </c>
       <c r="F6" t="n">
-        <v>434.8</v>
+        <v>448.24</v>
       </c>
       <c r="G6" t="n">
-        <v>-724.8</v>
+        <v>-710.24</v>
       </c>
     </row>
     <row r="7">
@@ -593,19 +593,19 @@
         <v>337.5</v>
       </c>
       <c r="C7" t="n">
-        <v>1502.5</v>
+        <v>1530.5</v>
       </c>
       <c r="D7" t="n">
-        <v>601</v>
+        <v>612.2</v>
       </c>
       <c r="E7" t="n">
-        <v>120.2</v>
+        <v>122.44</v>
       </c>
       <c r="F7" t="n">
-        <v>455.2</v>
+        <v>468.64</v>
       </c>
       <c r="G7" t="n">
-        <v>-702.7</v>
+        <v>-688.14</v>
       </c>
     </row>
     <row r="8">
@@ -616,19 +616,19 @@
         <v>345</v>
       </c>
       <c r="C8" t="n">
-        <v>1545</v>
+        <v>1573</v>
       </c>
       <c r="D8" t="n">
-        <v>618</v>
+        <v>629.2</v>
       </c>
       <c r="E8" t="n">
-        <v>123.6</v>
+        <v>125.84</v>
       </c>
       <c r="F8" t="n">
-        <v>475.6</v>
+        <v>489.04</v>
       </c>
       <c r="G8" t="n">
-        <v>-680.6</v>
+        <v>-666.04</v>
       </c>
     </row>
     <row r="9">
@@ -639,19 +639,19 @@
         <v>352.5</v>
       </c>
       <c r="C9" t="n">
-        <v>1587.5</v>
+        <v>1615.5</v>
       </c>
       <c r="D9" t="n">
-        <v>635</v>
+        <v>646.2</v>
       </c>
       <c r="E9" t="n">
-        <v>127</v>
+        <v>129.24</v>
       </c>
       <c r="F9" t="n">
-        <v>496</v>
+        <v>509.44</v>
       </c>
       <c r="G9" t="n">
-        <v>-658.5</v>
+        <v>-643.9400000000001</v>
       </c>
     </row>
     <row r="10">
@@ -662,19 +662,19 @@
         <v>360</v>
       </c>
       <c r="C10" t="n">
-        <v>1630</v>
+        <v>1658</v>
       </c>
       <c r="D10" t="n">
-        <v>652</v>
+        <v>663.2</v>
       </c>
       <c r="E10" t="n">
-        <v>130.4</v>
+        <v>132.64</v>
       </c>
       <c r="F10" t="n">
-        <v>516.4</v>
+        <v>529.84</v>
       </c>
       <c r="G10" t="n">
-        <v>-636.4</v>
+        <v>-621.84</v>
       </c>
     </row>
     <row r="11">
@@ -685,19 +685,19 @@
         <v>367.5</v>
       </c>
       <c r="C11" t="n">
-        <v>1672.5</v>
+        <v>1700.5</v>
       </c>
       <c r="D11" t="n">
-        <v>669</v>
+        <v>680.2</v>
       </c>
       <c r="E11" t="n">
-        <v>133.8</v>
+        <v>136.04</v>
       </c>
       <c r="F11" t="n">
-        <v>536.8</v>
+        <v>550.24</v>
       </c>
       <c r="G11" t="n">
-        <v>-614.3</v>
+        <v>-599.74</v>
       </c>
     </row>
     <row r="12">
@@ -708,19 +708,19 @@
         <v>375</v>
       </c>
       <c r="C12" t="n">
-        <v>1715</v>
+        <v>1743</v>
       </c>
       <c r="D12" t="n">
-        <v>686</v>
+        <v>697.2</v>
       </c>
       <c r="E12" t="n">
-        <v>137.2</v>
+        <v>139.44</v>
       </c>
       <c r="F12" t="n">
-        <v>557.2</v>
+        <v>570.64</v>
       </c>
       <c r="G12" t="n">
-        <v>-592.2</v>
+        <v>-577.64</v>
       </c>
     </row>
     <row r="13">
@@ -731,19 +731,19 @@
         <v>382.5</v>
       </c>
       <c r="C13" t="n">
-        <v>1757.5</v>
+        <v>1785.5</v>
       </c>
       <c r="D13" t="n">
-        <v>703</v>
+        <v>714.2</v>
       </c>
       <c r="E13" t="n">
-        <v>140.6</v>
+        <v>142.84</v>
       </c>
       <c r="F13" t="n">
-        <v>577.6</v>
+        <v>591.04</v>
       </c>
       <c r="G13" t="n">
-        <v>-570.1</v>
+        <v>-555.54</v>
       </c>
     </row>
     <row r="14">
@@ -754,19 +754,19 @@
         <v>390</v>
       </c>
       <c r="C14" t="n">
-        <v>1800</v>
+        <v>1828</v>
       </c>
       <c r="D14" t="n">
-        <v>720</v>
+        <v>731.2</v>
       </c>
       <c r="E14" t="n">
-        <v>144</v>
+        <v>146.24</v>
       </c>
       <c r="F14" t="n">
-        <v>598</v>
+        <v>611.4400000000001</v>
       </c>
       <c r="G14" t="n">
-        <v>-548</v>
+        <v>-533.4400000000001</v>
       </c>
     </row>
     <row r="15">
@@ -777,157 +777,19 @@
         <v>397.5</v>
       </c>
       <c r="C15" t="n">
-        <v>1842.5</v>
+        <v>1870.5</v>
       </c>
       <c r="D15" t="n">
-        <v>737</v>
+        <v>748.2</v>
       </c>
       <c r="E15" t="n">
-        <v>147.4</v>
+        <v>149.64</v>
       </c>
       <c r="F15" t="n">
-        <v>618.4</v>
+        <v>631.84</v>
       </c>
       <c r="G15" t="n">
-        <v>-525.9</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>2700</v>
-      </c>
-      <c r="B16" t="n">
-        <v>405</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1885</v>
-      </c>
-      <c r="D16" t="n">
-        <v>754</v>
-      </c>
-      <c r="E16" t="n">
-        <v>150.8</v>
-      </c>
-      <c r="F16" t="n">
-        <v>638.8</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-503.8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>2750</v>
-      </c>
-      <c r="B17" t="n">
-        <v>412.5</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1927.5</v>
-      </c>
-      <c r="D17" t="n">
-        <v>771</v>
-      </c>
-      <c r="E17" t="n">
-        <v>154.2</v>
-      </c>
-      <c r="F17" t="n">
-        <v>659.2</v>
-      </c>
-      <c r="G17" t="n">
-        <v>-481.7</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>2800</v>
-      </c>
-      <c r="B18" t="n">
-        <v>420</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1970</v>
-      </c>
-      <c r="D18" t="n">
-        <v>788</v>
-      </c>
-      <c r="E18" t="n">
-        <v>157.6</v>
-      </c>
-      <c r="F18" t="n">
-        <v>679.6</v>
-      </c>
-      <c r="G18" t="n">
-        <v>-459.6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2850</v>
-      </c>
-      <c r="B19" t="n">
-        <v>427.5</v>
-      </c>
-      <c r="C19" t="n">
-        <v>2012.5</v>
-      </c>
-      <c r="D19" t="n">
-        <v>805</v>
-      </c>
-      <c r="E19" t="n">
-        <v>161</v>
-      </c>
-      <c r="F19" t="n">
-        <v>700</v>
-      </c>
-      <c r="G19" t="n">
-        <v>-437.5</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>2900</v>
-      </c>
-      <c r="B20" t="n">
-        <v>435</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2055</v>
-      </c>
-      <c r="D20" t="n">
-        <v>822</v>
-      </c>
-      <c r="E20" t="n">
-        <v>164.4</v>
-      </c>
-      <c r="F20" t="n">
-        <v>720.4</v>
-      </c>
-      <c r="G20" t="n">
-        <v>-415.4</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>2950</v>
-      </c>
-      <c r="B21" t="n">
-        <v>442.5</v>
-      </c>
-      <c r="C21" t="n">
-        <v>2097.5</v>
-      </c>
-      <c r="D21" t="n">
-        <v>839</v>
-      </c>
-      <c r="E21" t="n">
-        <v>167.8</v>
-      </c>
-      <c r="F21" t="n">
-        <v>740.8</v>
-      </c>
-      <c r="G21" t="n">
-        <v>-393.3</v>
+        <v>-511.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor rent sensitivity calculations and update rent levels range
</commit_message>
<xml_diff>
--- a/rent_sensitivity_barking_riverside.xlsx
+++ b/rent_sensitivity_barking_riverside.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,327 +469,478 @@
           <t>Net Monthly Income (£)</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Savings vs Empty (£)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="B2" t="n">
-        <v>300</v>
+        <v>216</v>
       </c>
       <c r="C2" t="n">
-        <v>1318</v>
+        <v>1302</v>
       </c>
       <c r="D2" t="n">
-        <v>527.2</v>
+        <v>520.8</v>
       </c>
       <c r="E2" t="n">
-        <v>105.44</v>
+        <v>104.16</v>
       </c>
       <c r="F2" t="n">
-        <v>366.64</v>
+        <v>358.96</v>
       </c>
       <c r="G2" t="n">
-        <v>-798.64</v>
+        <v>-806.96</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1325.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2050</v>
+        <v>1850</v>
       </c>
       <c r="B3" t="n">
-        <v>307.5</v>
+        <v>222</v>
       </c>
       <c r="C3" t="n">
-        <v>1360.5</v>
+        <v>1346</v>
       </c>
       <c r="D3" t="n">
-        <v>544.2</v>
+        <v>538.4</v>
       </c>
       <c r="E3" t="n">
-        <v>108.84</v>
+        <v>107.68</v>
       </c>
       <c r="F3" t="n">
-        <v>387.04</v>
+        <v>380.08</v>
       </c>
       <c r="G3" t="n">
-        <v>-776.54</v>
+        <v>-784.08</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1347.92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="B4" t="n">
-        <v>315</v>
+        <v>228</v>
       </c>
       <c r="C4" t="n">
-        <v>1403</v>
+        <v>1390</v>
       </c>
       <c r="D4" t="n">
-        <v>561.2</v>
+        <v>556</v>
       </c>
       <c r="E4" t="n">
-        <v>112.24</v>
+        <v>111.2</v>
       </c>
       <c r="F4" t="n">
-        <v>407.44</v>
+        <v>401.2</v>
       </c>
       <c r="G4" t="n">
-        <v>-754.4400000000001</v>
+        <v>-761.2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1370.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2150</v>
+        <v>1950</v>
       </c>
       <c r="B5" t="n">
-        <v>322.5</v>
+        <v>234</v>
       </c>
       <c r="C5" t="n">
-        <v>1445.5</v>
+        <v>1434</v>
       </c>
       <c r="D5" t="n">
-        <v>578.2</v>
+        <v>573.6</v>
       </c>
       <c r="E5" t="n">
-        <v>115.64</v>
+        <v>114.72</v>
       </c>
       <c r="F5" t="n">
-        <v>427.84</v>
+        <v>422.32</v>
       </c>
       <c r="G5" t="n">
-        <v>-732.34</v>
+        <v>-738.3200000000001</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1393.68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2200</v>
+        <v>2000</v>
       </c>
       <c r="B6" t="n">
-        <v>330</v>
+        <v>240</v>
       </c>
       <c r="C6" t="n">
-        <v>1488</v>
+        <v>1478</v>
       </c>
       <c r="D6" t="n">
-        <v>595.2</v>
+        <v>591.2</v>
       </c>
       <c r="E6" t="n">
-        <v>119.04</v>
+        <v>118.24</v>
       </c>
       <c r="F6" t="n">
-        <v>448.24</v>
+        <v>443.44</v>
       </c>
       <c r="G6" t="n">
-        <v>-710.24</v>
+        <v>-715.4400000000001</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1416.56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2250</v>
+        <v>2050</v>
       </c>
       <c r="B7" t="n">
-        <v>337.5</v>
+        <v>246</v>
       </c>
       <c r="C7" t="n">
-        <v>1530.5</v>
+        <v>1522</v>
       </c>
       <c r="D7" t="n">
-        <v>612.2</v>
+        <v>608.8</v>
       </c>
       <c r="E7" t="n">
-        <v>122.44</v>
+        <v>121.76</v>
       </c>
       <c r="F7" t="n">
-        <v>468.64</v>
+        <v>464.56</v>
       </c>
       <c r="G7" t="n">
-        <v>-688.14</v>
+        <v>-692.5599999999999</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1439.44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2300</v>
+        <v>2100</v>
       </c>
       <c r="B8" t="n">
-        <v>345</v>
+        <v>252</v>
       </c>
       <c r="C8" t="n">
-        <v>1573</v>
+        <v>1566</v>
       </c>
       <c r="D8" t="n">
-        <v>629.2</v>
+        <v>626.4</v>
       </c>
       <c r="E8" t="n">
-        <v>125.84</v>
+        <v>125.28</v>
       </c>
       <c r="F8" t="n">
-        <v>489.04</v>
+        <v>485.68</v>
       </c>
       <c r="G8" t="n">
-        <v>-666.04</v>
+        <v>-669.6799999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1462.32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2350</v>
+        <v>2150</v>
       </c>
       <c r="B9" t="n">
-        <v>352.5</v>
+        <v>258</v>
       </c>
       <c r="C9" t="n">
-        <v>1615.5</v>
+        <v>1610</v>
       </c>
       <c r="D9" t="n">
-        <v>646.2</v>
+        <v>644</v>
       </c>
       <c r="E9" t="n">
-        <v>129.24</v>
+        <v>128.8</v>
       </c>
       <c r="F9" t="n">
-        <v>509.44</v>
+        <v>506.8</v>
       </c>
       <c r="G9" t="n">
-        <v>-643.9400000000001</v>
+        <v>-646.8</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1485.2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2400</v>
+        <v>2200</v>
       </c>
       <c r="B10" t="n">
-        <v>360</v>
+        <v>264</v>
       </c>
       <c r="C10" t="n">
-        <v>1658</v>
+        <v>1654</v>
       </c>
       <c r="D10" t="n">
-        <v>663.2</v>
+        <v>661.6</v>
       </c>
       <c r="E10" t="n">
-        <v>132.64</v>
+        <v>132.32</v>
       </c>
       <c r="F10" t="n">
-        <v>529.84</v>
+        <v>527.92</v>
       </c>
       <c r="G10" t="n">
-        <v>-621.84</v>
+        <v>-623.92</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1508.08</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2450</v>
+        <v>2250</v>
       </c>
       <c r="B11" t="n">
-        <v>367.5</v>
+        <v>270</v>
       </c>
       <c r="C11" t="n">
-        <v>1700.5</v>
+        <v>1698</v>
       </c>
       <c r="D11" t="n">
-        <v>680.2</v>
+        <v>679.2</v>
       </c>
       <c r="E11" t="n">
-        <v>136.04</v>
+        <v>135.84</v>
       </c>
       <c r="F11" t="n">
-        <v>550.24</v>
+        <v>549.04</v>
       </c>
       <c r="G11" t="n">
-        <v>-599.74</v>
+        <v>-601.04</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1530.96</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2500</v>
+        <v>2300</v>
       </c>
       <c r="B12" t="n">
-        <v>375</v>
+        <v>276</v>
       </c>
       <c r="C12" t="n">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D12" t="n">
-        <v>697.2</v>
+        <v>696.8</v>
       </c>
       <c r="E12" t="n">
-        <v>139.44</v>
+        <v>139.36</v>
       </c>
       <c r="F12" t="n">
-        <v>570.64</v>
+        <v>570.16</v>
       </c>
       <c r="G12" t="n">
-        <v>-577.64</v>
+        <v>-578.16</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1553.84</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2550</v>
+        <v>2350</v>
       </c>
       <c r="B13" t="n">
-        <v>382.5</v>
+        <v>282</v>
       </c>
       <c r="C13" t="n">
-        <v>1785.5</v>
+        <v>1786</v>
       </c>
       <c r="D13" t="n">
-        <v>714.2</v>
+        <v>714.4</v>
       </c>
       <c r="E13" t="n">
-        <v>142.84</v>
+        <v>142.88</v>
       </c>
       <c r="F13" t="n">
-        <v>591.04</v>
+        <v>591.28</v>
       </c>
       <c r="G13" t="n">
-        <v>-555.54</v>
+        <v>-555.28</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1576.72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2600</v>
+        <v>2400</v>
       </c>
       <c r="B14" t="n">
-        <v>390</v>
+        <v>288</v>
       </c>
       <c r="C14" t="n">
-        <v>1828</v>
+        <v>1830</v>
       </c>
       <c r="D14" t="n">
-        <v>731.2</v>
+        <v>732</v>
       </c>
       <c r="E14" t="n">
-        <v>146.24</v>
+        <v>146.4</v>
       </c>
       <c r="F14" t="n">
-        <v>611.4400000000001</v>
+        <v>612.4</v>
       </c>
       <c r="G14" t="n">
-        <v>-533.4400000000001</v>
+        <v>-532.4</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1599.6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>2450</v>
+      </c>
+      <c r="B15" t="n">
+        <v>294</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1874</v>
+      </c>
+      <c r="D15" t="n">
+        <v>749.6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>149.92</v>
+      </c>
+      <c r="F15" t="n">
+        <v>633.52</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-509.52</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1622.48</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="B16" t="n">
+        <v>300</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1918</v>
+      </c>
+      <c r="D16" t="n">
+        <v>767.2</v>
+      </c>
+      <c r="E16" t="n">
+        <v>153.44</v>
+      </c>
+      <c r="F16" t="n">
+        <v>654.64</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-486.64</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1645.36</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2550</v>
+      </c>
+      <c r="B17" t="n">
+        <v>306</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1962</v>
+      </c>
+      <c r="D17" t="n">
+        <v>784.8</v>
+      </c>
+      <c r="E17" t="n">
+        <v>156.96</v>
+      </c>
+      <c r="F17" t="n">
+        <v>675.76</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-463.76</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1668.24</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2600</v>
+      </c>
+      <c r="B18" t="n">
+        <v>312</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2006</v>
+      </c>
+      <c r="D18" t="n">
+        <v>802.4</v>
+      </c>
+      <c r="E18" t="n">
+        <v>160.48</v>
+      </c>
+      <c r="F18" t="n">
+        <v>696.88</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-440.88</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1691.12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>2650</v>
       </c>
-      <c r="B15" t="n">
-        <v>397.5</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1870.5</v>
-      </c>
-      <c r="D15" t="n">
-        <v>748.2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>149.64</v>
-      </c>
-      <c r="F15" t="n">
-        <v>631.84</v>
-      </c>
-      <c r="G15" t="n">
-        <v>-511.34</v>
+      <c r="B19" t="n">
+        <v>318</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2050</v>
+      </c>
+      <c r="D19" t="n">
+        <v>820</v>
+      </c>
+      <c r="E19" t="n">
+        <v>164</v>
+      </c>
+      <c r="F19" t="n">
+        <v>718</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-418</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>